<commit_message>
Implemented First Review Changes
</commit_message>
<xml_diff>
--- a/Hardware/Electronics/Time Circuit Control/BOM/BOM_PCBWay.xlsx
+++ b/Hardware/Electronics/Time Circuit Control/BOM/BOM_PCBWay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\Time Circuit Project\Hardware\Electronics\Time Circuit Control\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054243DC-E7CA-4BF0-BA9E-BD4C760CB413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC4925F-AE75-4CA2-93CF-3CCC64560979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,24 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="175">
   <si>
     <t>Item #</t>
   </si>
@@ -195,9 +207,6 @@
     <t>J9</t>
   </si>
   <si>
-    <t>J10, J11</t>
-  </si>
-  <si>
     <t>L1, L2</t>
   </si>
   <si>
@@ -210,9 +219,6 @@
     <t>Q1, Q2, Q3, Q4, Q5</t>
   </si>
   <si>
-    <t>R1, R8, R9, R12, R35, R36</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -222,15 +228,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>R10, R11, R17, R18, R19, R20, R23, R24, R25, R26</t>
-  </si>
-  <si>
-    <t>R21, R22, R27, R28</t>
-  </si>
-  <si>
-    <t>R29, R30, R31, R32, R33, R34</t>
-  </si>
-  <si>
     <t>RN1</t>
   </si>
   <si>
@@ -594,12 +591,6 @@
     <t>Thick Film Resistors - SMD 1/2watt 120ohm 1% High Power AEC-Q200</t>
   </si>
   <si>
-    <t>R16, R7</t>
-  </si>
-  <si>
-    <t>R13, R14, R15, R6</t>
-  </si>
-  <si>
     <t>CRCW0805150RFKEAHP</t>
   </si>
   <si>
@@ -610,18 +601,55 @@
   </si>
   <si>
     <t>Thick Film Resistors - SMD 1/2watt 150ohms 1% High Power AEC-Q200</t>
+  </si>
+  <si>
+    <t>R1, R8, R9, R12, R39, R40</t>
+  </si>
+  <si>
+    <t>R10, R11, R17, R18, R19, R20, R25, R26 ,R27, R28</t>
+  </si>
+  <si>
+    <t>R21, R22, R23, R24, R29, R30, R31, R32</t>
+  </si>
+  <si>
+    <t>R33, R34, R35, R36, R37, R38</t>
+  </si>
+  <si>
+    <t>R6, R13, R14, R15</t>
+  </si>
+  <si>
+    <t>R7, R16</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11, J12</t>
+  </si>
+  <si>
+    <t>M20-9990345</t>
+  </si>
+  <si>
+    <t>HDRV3W64P0X254_1X3_762X254X864P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -752,53 +780,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -808,38 +830,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1193,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I50"/>
+  <dimension ref="A2:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1207,32 +1244,32 @@
     <col min="4" max="4" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="85.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" style="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="35.5703125" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="D2" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="D2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1253,7 +1290,7 @@
       <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="25" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -1267,22 +1304,22 @@
       <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" s="16">
+      <c r="B7" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="14">
         <v>16</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -1294,22 +1331,22 @@
       <c r="A8" s="10">
         <v>2</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="14">
         <v>1</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="G8" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -1321,22 +1358,22 @@
       <c r="A9" s="7">
         <v>3</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <v>2</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="G9" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -1348,22 +1385,22 @@
       <c r="A10" s="10">
         <v>4</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="14">
         <v>3</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -1375,22 +1412,22 @@
       <c r="A11" s="7">
         <v>5</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <v>1</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G11" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -1402,22 +1439,22 @@
       <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <v>1</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -1429,23 +1466,23 @@
       <c r="A13" s="7">
         <v>7</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <v>1</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>9</v>
@@ -1456,22 +1493,22 @@
       <c r="A14" s="10">
         <v>8</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <v>1</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14" s="24">
+        <v>117</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="22">
         <v>2020</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -1483,23 +1520,23 @@
       <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="14">
         <v>2</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>125</v>
+        <v>132</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>9</v>
@@ -1510,23 +1547,23 @@
       <c r="A16" s="10">
         <v>10</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="14">
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>126</v>
+        <v>136</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>9</v>
@@ -1537,23 +1574,23 @@
       <c r="A17" s="7">
         <v>11</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="14">
         <v>1</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>130</v>
+        <v>135</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>125</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>9</v>
@@ -1564,23 +1601,23 @@
       <c r="A18" s="10">
         <v>12</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="14">
         <v>1</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>132</v>
+        <v>134</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>127</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>9</v>
@@ -1591,23 +1628,23 @@
       <c r="A19" s="7">
         <v>13</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="14">
         <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>134</v>
+      <c r="E19" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>9</v>
@@ -1618,23 +1655,23 @@
       <c r="A20" s="10">
         <v>14</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="14">
         <v>1</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>130</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>9</v>
@@ -1645,810 +1682,833 @@
       <c r="A21" s="7">
         <v>15</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="14">
         <v>2</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="18" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="23" t="s">
-        <v>111</v>
+      <c r="I21" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15">
       <c r="A22" s="10">
         <v>16</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="14">
         <v>2</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" s="17" t="s">
+      <c r="D22" s="16"/>
+      <c r="E22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="23" t="s">
-        <v>111</v>
+      <c r="I22" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15">
       <c r="A23" s="7">
         <v>17</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="16">
-        <v>1</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H23" s="18" t="s">
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="23" t="s">
-        <v>111</v>
+      <c r="I23" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15">
       <c r="A24" s="10">
         <v>18</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="16">
-        <v>1</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="H24" s="18" t="s">
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="23" t="s">
-        <v>111</v>
+      <c r="I24" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" ht="15">
       <c r="A25" s="7">
         <v>19</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="16">
-        <v>1</v>
-      </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="18" t="s">
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="23" t="s">
-        <v>111</v>
+      <c r="I25" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15">
       <c r="A26" s="10">
         <v>20</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="16">
-        <v>1</v>
-      </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="H26" s="18" t="s">
+      <c r="C26" s="14">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="23" t="s">
-        <v>111</v>
+      <c r="I26" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15">
       <c r="A27" s="7">
         <v>21</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="16">
-        <v>1</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="C27" s="14">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="10">
         <v>22</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="16">
-        <v>2</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" s="18" t="s">
+      <c r="B28" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="23" t="s">
-        <v>111</v>
+      <c r="I28" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15">
       <c r="A29" s="7">
         <v>23</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="16">
+      <c r="B29" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="14">
         <v>2</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="18"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="15">
       <c r="A30" s="10">
         <v>24</v>
       </c>
-      <c r="B30" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="16">
+      <c r="B30" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="14">
         <v>2</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="18"/>
+      <c r="D30" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="16"/>
     </row>
     <row r="31" spans="1:9" ht="15">
       <c r="A31" s="7">
         <v>25</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="16">
-        <v>4</v>
-      </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="B31" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="14">
+        <v>2</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="16"/>
     </row>
     <row r="32" spans="1:9" ht="15">
       <c r="A32" s="10">
         <v>26</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="16">
-        <v>5</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="18"/>
+      <c r="B32" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="14">
+        <v>4</v>
+      </c>
+      <c r="D32" s="16"/>
+      <c r="E32" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="15">
       <c r="A33" s="7">
         <v>27</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="16">
-        <v>6</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I33" s="18"/>
+      <c r="B33" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="14">
+        <v>5</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="16"/>
     </row>
     <row r="34" spans="1:9" ht="15">
       <c r="A34" s="10">
         <v>28</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="16">
-        <v>1</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F34" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="G34" s="25" t="s">
+      <c r="B34" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="14">
+        <v>6</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I34" s="18"/>
+      <c r="H34" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="16"/>
     </row>
     <row r="35" spans="1:9" ht="15">
       <c r="A35" s="7">
         <v>29</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="16">
-        <v>2</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="G35" s="25" t="s">
+      <c r="B35" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="14">
+        <v>1</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I35" s="18"/>
+      <c r="H35" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="16"/>
     </row>
     <row r="36" spans="1:9" ht="15">
       <c r="A36" s="10">
         <v>30</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="16">
-        <v>1</v>
-      </c>
-      <c r="D36" s="18" t="s">
+      <c r="B36" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="14">
+        <v>2</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="E36" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="G36" s="25" t="s">
+      <c r="G36" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I36" s="18"/>
-    </row>
-    <row r="37" spans="1:9" ht="30">
+      <c r="H36" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="16"/>
+    </row>
+    <row r="37" spans="1:9" ht="15">
       <c r="A37" s="7">
         <v>31</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="16">
-        <v>10</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="G37" s="25" t="s">
+      <c r="B37" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="14">
+        <v>1</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I37" s="18"/>
-    </row>
-    <row r="38" spans="1:9" ht="15">
+      <c r="H37" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="16"/>
+    </row>
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="10">
         <v>32</v>
       </c>
-      <c r="B38" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="16">
-        <v>4</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="F38" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="G38" s="25" t="s">
+      <c r="B38" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="14">
+        <v>10</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="G38" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I38" s="18"/>
+      <c r="H38" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" ht="15">
       <c r="A39" s="7">
         <v>33</v>
       </c>
-      <c r="B39" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="C39" s="16">
-        <v>2</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E39" s="22" t="s">
+      <c r="B39" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="F39" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="G39" s="25" t="s">
+      <c r="C39" s="14">
+        <v>4</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G39" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I39" s="18"/>
+      <c r="H39" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="16"/>
     </row>
     <row r="40" spans="1:9" ht="15">
       <c r="A40" s="10">
         <v>34</v>
       </c>
-      <c r="B40" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="16">
-        <v>4</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="G40" s="25" t="s">
+      <c r="B40" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="14">
+        <v>2</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="G40" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I40" s="18"/>
+      <c r="H40" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="16"/>
     </row>
     <row r="41" spans="1:9" ht="30">
       <c r="A41" s="7">
         <v>35</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="16">
-        <v>6</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="F41" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="G41" s="25" t="s">
+      <c r="B41" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="14">
+        <v>8</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="18"/>
-    </row>
-    <row r="42" spans="1:9" ht="15">
+      <c r="H41" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="1:9" ht="30">
       <c r="A42" s="10">
         <v>36</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="16">
-        <v>1</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42" s="18"/>
+      <c r="B42" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="14">
+        <v>6</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="16"/>
     </row>
     <row r="43" spans="1:9" ht="15">
       <c r="A43" s="7">
         <v>37</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="16">
-        <v>2</v>
-      </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="B43" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="14">
+        <v>1</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:9" ht="15">
       <c r="A44" s="10">
         <v>38</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="16">
-        <v>1</v>
-      </c>
-      <c r="D44" s="18"/>
-      <c r="E44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G44" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H44" s="18" t="s">
+      <c r="B44" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="14">
+        <v>2</v>
+      </c>
+      <c r="D44" s="16"/>
+      <c r="E44" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="23" t="s">
-        <v>111</v>
+      <c r="I44" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15">
       <c r="A45" s="7">
         <v>39</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="16">
-        <v>1</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I45" s="18"/>
+      <c r="B45" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="14">
+        <v>1</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="46" spans="1:9" ht="15">
       <c r="A46" s="10">
         <v>40</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="16">
-        <v>1</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G46" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="23" t="s">
-        <v>111</v>
-      </c>
+      <c r="B46" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="14">
+        <v>1</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" s="16"/>
     </row>
     <row r="47" spans="1:9" ht="15">
       <c r="A47" s="7">
         <v>41</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="16">
-        <v>1</v>
-      </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="24" t="s">
+      <c r="B47" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="14">
+        <v>1</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="21" t="s">
         <v>106</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" s="23" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15">
       <c r="A48" s="10">
         <v>42</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="16">
-        <v>1</v>
-      </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="17" t="s">
+      <c r="B48" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="14">
+        <v>1</v>
+      </c>
+      <c r="D48" s="16"/>
+      <c r="E48" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F48" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="H48" s="18" t="s">
+      <c r="G48" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="H48" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I48" s="23" t="s">
-        <v>111</v>
+      <c r="I48" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15">
       <c r="A49" s="7">
         <v>43</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="16">
-        <v>1</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="G49" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I49" s="18"/>
+      <c r="B49" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="14">
+        <v>1</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="21" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="50" spans="1:9" ht="15">
       <c r="A50" s="10">
         <v>44</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="16">
-        <v>1</v>
-      </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G50" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="H50" s="18" t="s">
+      <c r="B50" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="14">
+        <v>1</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" s="16"/>
+    </row>
+    <row r="51" spans="1:9" ht="15">
+      <c r="A51" s="7">
+        <v>45</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="14">
+        <v>1</v>
+      </c>
+      <c r="D51" s="16"/>
+      <c r="E51" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H51" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I50" s="23" t="s">
-        <v>111</v>
+      <c r="I51" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2456,7 +2516,7 @@
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Minor Changes/ Ready for Release
</commit_message>
<xml_diff>
--- a/Hardware/Electronics/Time Circuit Control/BOM/BOM_PCBWay.xlsx
+++ b/Hardware/Electronics/Time Circuit Control/BOM/BOM_PCBWay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\Time Circuit Project\Hardware\Electronics\Time Circuit Control\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC4925F-AE75-4CA2-93CF-3CCC64560979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD2C53-7EB6-4E33-9E87-21E718F75A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="181">
   <si>
     <t>Item #</t>
   </si>
@@ -632,17 +632,42 @@
   <si>
     <t>HDRV3W64P0X254_1X3_762X254X864P</t>
   </si>
+  <si>
+    <t>CTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Harwin</t>
+  </si>
+  <si>
+    <t>Coin Cell Battery Holders EZ BDWR, SMT COIN CELL HOLDER CR2032</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>Memory Card Connectors Micro SD Push-Push, SMT, 1.40mm Profile, With Peg, Open Switch, T&amp;R</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -780,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -789,38 +814,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -830,53 +855,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1233,7 +1258,7 @@
   <dimension ref="A2:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1244,32 +1269,32 @@
     <col min="4" max="4" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="85.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" style="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="35.5703125" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="D2" s="27" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="D2" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1290,7 +1315,7 @@
       <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -1304,7 +1329,7 @@
       <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>158</v>
       </c>
       <c r="C7" s="14">
@@ -1313,13 +1338,13 @@
       <c r="D7" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -1340,13 +1365,13 @@
       <c r="D8" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -1367,13 +1392,13 @@
       <c r="D9" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -1394,13 +1419,13 @@
       <c r="D10" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -1421,13 +1446,13 @@
       <c r="D11" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -1448,13 +1473,13 @@
       <c r="D12" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -1475,13 +1500,13 @@
       <c r="D13" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>114</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -1502,13 +1527,13 @@
       <c r="D14" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="21">
         <v>2020</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -1529,13 +1554,13 @@
       <c r="D15" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="22" t="s">
         <v>120</v>
       </c>
       <c r="H15" s="9" t="s">
@@ -1556,13 +1581,13 @@
       <c r="D16" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="22" t="s">
         <v>121</v>
       </c>
       <c r="H16" s="9" t="s">
@@ -1583,13 +1608,13 @@
       <c r="D17" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="22" t="s">
         <v>125</v>
       </c>
       <c r="H17" s="9" t="s">
@@ -1610,13 +1635,13 @@
       <c r="D18" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="22" t="s">
         <v>127</v>
       </c>
       <c r="H18" s="9" t="s">
@@ -1637,13 +1662,13 @@
       <c r="D19" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="22" t="s">
         <v>129</v>
       </c>
       <c r="H19" s="9" t="s">
@@ -1664,13 +1689,13 @@
       <c r="D20" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="22" t="s">
         <v>130</v>
       </c>
       <c r="H20" s="9" t="s">
@@ -1689,19 +1714,19 @@
         <v>2</v>
       </c>
       <c r="D21" s="16"/>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="31" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="21" t="s">
         <v>91</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="I21" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1716,19 +1741,19 @@
         <v>2</v>
       </c>
       <c r="D22" s="16"/>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="31" t="s">
         <v>63</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="21" t="s">
         <v>92</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1742,22 +1767,22 @@
       <c r="C23" s="14">
         <v>1</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="15" t="s">
+      <c r="D23" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="22" t="s">
+      <c r="F23" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="G23" s="21" t="s">
         <v>93</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>106</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="15">
       <c r="A24" s="10">
@@ -1769,20 +1794,20 @@
       <c r="C24" s="14">
         <v>1</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="15" t="s">
+      <c r="D24" s="17"/>
+      <c r="E24" s="31" t="s">
         <v>65</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="21" t="s">
         <v>94</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1796,20 +1821,20 @@
       <c r="C25" s="14">
         <v>1</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="15" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="31" t="s">
         <v>66</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="21" t="s">
         <v>66</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1823,97 +1848,101 @@
       <c r="C26" s="14">
         <v>1</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="15" t="s">
+      <c r="D26" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="22" t="s">
+      <c r="F26" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="G26" s="21" t="s">
         <v>95</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>106</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" spans="1:9" ht="15">
       <c r="A27" s="7">
         <v>21</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="14">
         <v>1</v>
       </c>
       <c r="D27" s="16"/>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="31" t="s">
         <v>173</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="21"/>
+      <c r="H27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="10">
         <v>22</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>171</v>
       </c>
       <c r="C28" s="14">
         <v>1</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="15" t="s">
+      <c r="D28" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="31" t="s">
         <v>68</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="21" t="s">
         <v>96</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>106</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="15">
       <c r="A29" s="7">
         <v>23</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="27" t="s">
         <v>172</v>
       </c>
       <c r="C29" s="14">
         <v>2</v>
       </c>
       <c r="D29" s="16"/>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="31" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="21" t="s">
         <v>97</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="21" t="s">
+      <c r="I29" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1930,13 +1959,13 @@
       <c r="D30" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="16" t="s">
@@ -1957,13 +1986,13 @@
       <c r="D31" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="22" t="s">
         <v>142</v>
       </c>
       <c r="H31" s="16" t="s">
@@ -1988,13 +2017,13 @@
       <c r="F32" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="21" t="s">
         <v>71</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="21" t="s">
+      <c r="I32" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2011,13 +2040,13 @@
       <c r="D33" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="G33" s="23" t="s">
+      <c r="G33" s="22" t="s">
         <v>120</v>
       </c>
       <c r="H33" s="16" t="s">
@@ -2029,7 +2058,7 @@
       <c r="A34" s="10">
         <v>28</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="27" t="s">
         <v>165</v>
       </c>
       <c r="C34" s="14">
@@ -2038,13 +2067,13 @@
       <c r="D34" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="29" t="s">
+      <c r="F34" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G34" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H34" s="16" t="s">
@@ -2065,13 +2094,13 @@
       <c r="D35" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G35" s="23" t="s">
+      <c r="G35" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="16" t="s">
@@ -2092,13 +2121,13 @@
       <c r="D36" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="G36" s="23" t="s">
+      <c r="G36" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="16" t="s">
@@ -2119,13 +2148,13 @@
       <c r="D37" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="G37" s="23" t="s">
+      <c r="G37" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="16" t="s">
@@ -2137,7 +2166,7 @@
       <c r="A38" s="10">
         <v>32</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="27" t="s">
         <v>166</v>
       </c>
       <c r="C38" s="14">
@@ -2146,13 +2175,13 @@
       <c r="D38" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G38" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="16" t="s">
@@ -2164,7 +2193,7 @@
       <c r="A39" s="7">
         <v>33</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="27" t="s">
         <v>169</v>
       </c>
       <c r="C39" s="14">
@@ -2173,13 +2202,13 @@
       <c r="D39" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="16" t="s">
@@ -2191,7 +2220,7 @@
       <c r="A40" s="10">
         <v>34</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="27" t="s">
         <v>170</v>
       </c>
       <c r="C40" s="14">
@@ -2200,13 +2229,13 @@
       <c r="D40" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G40" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="16" t="s">
@@ -2218,7 +2247,7 @@
       <c r="A41" s="7">
         <v>35</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="27" t="s">
         <v>167</v>
       </c>
       <c r="C41" s="14">
@@ -2227,13 +2256,13 @@
       <c r="D41" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G41" s="23" t="s">
+      <c r="G41" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="16" t="s">
@@ -2245,7 +2274,7 @@
       <c r="A42" s="10">
         <v>36</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="27" t="s">
         <v>168</v>
       </c>
       <c r="C42" s="14">
@@ -2254,13 +2283,13 @@
       <c r="D42" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="G42" s="23" t="s">
+      <c r="G42" s="22" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="16" t="s">
@@ -2281,13 +2310,13 @@
       <c r="D43" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="E43" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G43" s="23" t="s">
+      <c r="G43" s="22" t="s">
         <v>153</v>
       </c>
       <c r="H43" s="16" t="s">
@@ -2306,19 +2335,19 @@
         <v>2</v>
       </c>
       <c r="D44" s="16"/>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="31" t="s">
         <v>79</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="G44" s="21" t="s">
         <v>79</v>
       </c>
       <c r="H44" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="21" t="s">
+      <c r="I44" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2333,19 +2362,19 @@
         <v>1</v>
       </c>
       <c r="D45" s="16"/>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="31" t="s">
         <v>80</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G45" s="22" t="s">
+      <c r="G45" s="21" t="s">
         <v>98</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21" t="s">
+      <c r="I45" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2362,13 +2391,13 @@
       <c r="D46" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="E46" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="G46" s="21" t="s">
         <v>99</v>
       </c>
       <c r="H46" s="16" t="s">
@@ -2386,22 +2415,22 @@
       <c r="C47" s="14">
         <v>1</v>
       </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="15" t="s">
+      <c r="D47" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" s="31" t="s">
         <v>82</v>
       </c>
       <c r="F47" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G47" s="21" t="s">
         <v>100</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>106</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I47" s="16"/>
     </row>
     <row r="48" spans="1:9" ht="15">
       <c r="A48" s="10">
@@ -2414,19 +2443,19 @@
         <v>1</v>
       </c>
       <c r="D48" s="16"/>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="31" t="s">
         <v>83</v>
       </c>
       <c r="F48" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G48" s="22" t="s">
+      <c r="G48" s="21" t="s">
         <v>101</v>
       </c>
       <c r="H48" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I48" s="21" t="s">
+      <c r="I48" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2441,19 +2470,19 @@
         <v>1</v>
       </c>
       <c r="D49" s="16"/>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="31" t="s">
         <v>84</v>
       </c>
       <c r="F49" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G49" s="22" t="s">
+      <c r="G49" s="21" t="s">
         <v>102</v>
       </c>
       <c r="H49" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="21" t="s">
+      <c r="I49" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2470,13 +2499,13 @@
       <c r="D50" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E50" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F50" s="20" t="s">
+      <c r="F50" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="G50" s="22" t="s">
+      <c r="G50" s="21" t="s">
         <v>103</v>
       </c>
       <c r="H50" s="16" t="s">
@@ -2501,13 +2530,13 @@
       <c r="F51" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G51" s="22" t="s">
+      <c r="G51" s="21" t="s">
         <v>104</v>
       </c>
       <c r="H51" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I51" s="21" t="s">
+      <c r="I51" s="20" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2516,7 +2545,7 @@
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
   <drawing r:id="rId1"/>

</xml_diff>